<commit_message>
Added neopixels to parts list
</commit_message>
<xml_diff>
--- a/hardware/parts.xlsx
+++ b/hardware/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">LED strip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://onecall.farnell.com/mcm/25-7520/30-rgb-led-addressable-strip-1/dp/2801872?st=individually%20addressable%20rgb%20led%20strip</t>
   </si>
   <si>
     <t xml:space="preserve">Amplifier debounce capacitors</t>
@@ -216,13 +219,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -294,16 +297,16 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="88.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.1295546558705"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="88.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,7 +344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -433,19 +436,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>23.2</v>
+      </c>
       <c r="D9" s="1" t="n">
         <f aca="false">(B9*C9)</f>
-        <v>0</v>
+        <v>23.2</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -460,7 +471,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -473,12 +484,12 @@
         <v>26.26</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -493,7 +504,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>4</v>
@@ -506,12 +517,12 @@
         <v>2.412</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>4</v>
@@ -524,7 +535,7 @@
         <v>1.276</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,25 +649,26 @@
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">SUM(D2:D29)</f>
-        <v>57.704</v>
+        <v>80.904</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">100-D30</f>
-        <v>42.296</v>
+        <v>19.096</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://uk.rs-online.com/web/p/processor-microcontroller-development-kits/1438574/?relevancy-data=636F3D3126696E3D4931384E53656172636847656E65726963266C753D656E266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D31333326736E3D592673723D2673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432673633D592677633D4E4F4E45267573743D4E55434C454F2D4C3433324B43267374613D4E55434C454F2D4C3433324B4326&amp;searchHistory=%7B%22enabled%22%3Atrue%7D"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://onecall.farnell.com/microchip/mcp3301-ci-p/ic-13bit-adc-1ch-dip8-3301/dp/1332099"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>